<commit_message>
Marsframe work Sprint 2
</commit_message>
<xml_diff>
--- a/Mars Profile page Test Conditions and Test cases .xlsx
+++ b/Mars Profile page Test Conditions and Test cases .xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aswin\Desktop\Projects\marsframework\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CC8B106-DBA2-4412-8F23-0AEEAF05C34A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="45" windowWidth="5715" windowHeight="3930" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Mars Test Conditions" sheetId="1" r:id="rId1"/>
@@ -15,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="224">
   <si>
     <t>ID</t>
   </si>
@@ -1664,13 +1670,16 @@
       </rPr>
       <t xml:space="preserve"> Login with Valid Credentials Username: "lakshmi12_nlp@yahoo.com" and Password: "Abc@1234"</t>
     </r>
+  </si>
+  <si>
+    <t>ShareSkill</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1774,28 +1783,13 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1804,12 +1798,35 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1856,7 +1873,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1888,9 +1905,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1922,6 +1957,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2097,20 +2150,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D48"/>
   <sheetViews>
-    <sheetView topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="2" max="2" width="15.42578125" customWidth="1"/>
     <col min="3" max="3" width="40.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="69.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="6" customFormat="1">
+    <row r="1" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -2124,10 +2178,13 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>49</v>
       </c>
+      <c r="B2" t="s">
+        <v>223</v>
+      </c>
       <c r="C2" t="s">
         <v>7</v>
       </c>
@@ -2135,17 +2192,17 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>50</v>
       </c>
@@ -2156,7 +2213,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>51</v>
       </c>
@@ -2167,22 +2224,22 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D9" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D10" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D11" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>52</v>
       </c>
@@ -2193,12 +2250,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D14" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>53</v>
       </c>
@@ -2209,12 +2266,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D17" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>54</v>
       </c>
@@ -2225,12 +2282,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D20" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>55</v>
       </c>
@@ -2241,12 +2298,12 @@
         <v>41</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D23" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>56</v>
       </c>
@@ -2257,32 +2314,32 @@
         <v>26</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D26" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D27" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D28" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D29" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D30" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>57</v>
       </c>
@@ -2293,27 +2350,27 @@
         <v>25</v>
       </c>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D33" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D34" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="35" spans="1:4">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D35" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D36" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="38" spans="1:4">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>58</v>
       </c>
@@ -2324,27 +2381,27 @@
         <v>30</v>
       </c>
     </row>
-    <row r="39" spans="1:4">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D39" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="40" spans="1:4">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D40" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="41" spans="1:4">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D41" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="42" spans="1:4">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D42" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="44" spans="1:4">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>59</v>
       </c>
@@ -2355,22 +2412,22 @@
         <v>34</v>
       </c>
     </row>
-    <row r="45" spans="1:4">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D45" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="46" spans="1:4">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D46" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:4">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D47" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="48" spans="1:4">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D48" t="s">
         <v>37</v>
       </c>
@@ -2382,17 +2439,17 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z207"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A154" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A151" workbookViewId="0">
       <selection activeCell="E158" sqref="E158"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18" style="10" customWidth="1"/>
-    <col min="2" max="2" width="52" style="15" customWidth="1"/>
+    <col min="1" max="1" width="18" style="8" customWidth="1"/>
+    <col min="2" max="2" width="52" style="10" customWidth="1"/>
     <col min="3" max="3" width="55.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="24.28515625" customWidth="1"/>
     <col min="5" max="5" width="25.85546875" customWidth="1"/>
@@ -2401,11 +2458,11 @@
     <col min="8" max="8" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="21" customHeight="1" thickBot="1">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:26" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="9" t="s">
         <v>61</v>
       </c>
       <c r="C1" s="2" t="s">
@@ -2445,11 +2502,11 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="47.25" customHeight="1">
-      <c r="A2" s="9" t="s">
+    <row r="2" spans="1:26" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
         <v>68</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="15" t="s">
         <v>69</v>
       </c>
       <c r="C2" s="5" t="s">
@@ -2459,9 +2516,9 @@
         <v>76</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="45">
-      <c r="A3" s="7"/>
-      <c r="B3" s="14"/>
+    <row r="3" spans="1:26" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="12"/>
+      <c r="B3" s="16"/>
       <c r="C3" s="5" t="s">
         <v>71</v>
       </c>
@@ -2469,9 +2526,9 @@
         <v>77</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="30">
-      <c r="A4" s="7"/>
-      <c r="B4" s="14"/>
+    <row r="4" spans="1:26" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="12"/>
+      <c r="B4" s="16"/>
       <c r="C4" s="4" t="s">
         <v>72</v>
       </c>
@@ -2479,9 +2536,9 @@
         <v>79</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="30">
-      <c r="A5" s="7"/>
-      <c r="B5" s="14"/>
+    <row r="5" spans="1:26" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="12"/>
+      <c r="B5" s="16"/>
       <c r="C5" s="4" t="s">
         <v>73</v>
       </c>
@@ -2489,9 +2546,9 @@
         <v>80</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="45">
-      <c r="A6" s="7"/>
-      <c r="B6" s="14"/>
+    <row r="6" spans="1:26" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="12"/>
+      <c r="B6" s="16"/>
       <c r="C6" s="4" t="s">
         <v>74</v>
       </c>
@@ -2499,9 +2556,9 @@
         <v>78</v>
       </c>
     </row>
-    <row r="7" spans="1:26" ht="30">
-      <c r="A7" s="7"/>
-      <c r="B7" s="14"/>
+    <row r="7" spans="1:26" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="12"/>
+      <c r="B7" s="16"/>
       <c r="C7" s="4" t="s">
         <v>75</v>
       </c>
@@ -2509,14 +2566,14 @@
         <v>81</v>
       </c>
     </row>
-    <row r="8" spans="1:26">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="C8" s="4"/>
     </row>
-    <row r="9" spans="1:26" ht="45">
-      <c r="A9" s="7" t="s">
+    <row r="9" spans="1:26" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="B9" s="16" t="s">
+      <c r="B9" s="11" t="s">
         <v>5</v>
       </c>
       <c r="C9" s="5" t="s">
@@ -2526,9 +2583,9 @@
         <v>76</v>
       </c>
     </row>
-    <row r="10" spans="1:26" ht="45">
-      <c r="A10" s="7"/>
-      <c r="B10" s="16"/>
+    <row r="10" spans="1:26" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="12"/>
+      <c r="B10" s="11"/>
       <c r="C10" s="5" t="s">
         <v>71</v>
       </c>
@@ -2536,9 +2593,9 @@
         <v>77</v>
       </c>
     </row>
-    <row r="11" spans="1:26" ht="30">
-      <c r="A11" s="7"/>
-      <c r="B11" s="16"/>
+    <row r="11" spans="1:26" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="12"/>
+      <c r="B11" s="11"/>
       <c r="C11" s="4" t="s">
         <v>72</v>
       </c>
@@ -2546,9 +2603,9 @@
         <v>79</v>
       </c>
     </row>
-    <row r="12" spans="1:26" ht="30">
-      <c r="A12" s="7"/>
-      <c r="B12" s="16"/>
+    <row r="12" spans="1:26" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="12"/>
+      <c r="B12" s="11"/>
       <c r="C12" s="4" t="s">
         <v>73</v>
       </c>
@@ -2556,9 +2613,9 @@
         <v>80</v>
       </c>
     </row>
-    <row r="13" spans="1:26" ht="45">
-      <c r="A13" s="7"/>
-      <c r="B13" s="16"/>
+    <row r="13" spans="1:26" ht="45" x14ac:dyDescent="0.25">
+      <c r="A13" s="12"/>
+      <c r="B13" s="11"/>
       <c r="C13" s="4" t="s">
         <v>74</v>
       </c>
@@ -2566,9 +2623,9 @@
         <v>78</v>
       </c>
     </row>
-    <row r="14" spans="1:26" ht="30">
-      <c r="A14" s="7"/>
-      <c r="B14" s="16"/>
+    <row r="14" spans="1:26" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="12"/>
+      <c r="B14" s="11"/>
       <c r="C14" s="4" t="s">
         <v>75</v>
       </c>
@@ -2576,14 +2633,14 @@
         <v>81</v>
       </c>
     </row>
-    <row r="15" spans="1:26">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="C15" s="4"/>
     </row>
-    <row r="16" spans="1:26" ht="45">
-      <c r="A16" s="7" t="s">
+    <row r="16" spans="1:26" ht="45" x14ac:dyDescent="0.25">
+      <c r="A16" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="B16" s="16" t="s">
+      <c r="B16" s="11" t="s">
         <v>6</v>
       </c>
       <c r="C16" s="5" t="s">
@@ -2593,9 +2650,9 @@
         <v>76</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="45">
-      <c r="A17" s="7"/>
-      <c r="B17" s="16"/>
+    <row r="17" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A17" s="12"/>
+      <c r="B17" s="11"/>
       <c r="C17" s="5" t="s">
         <v>71</v>
       </c>
@@ -2603,9 +2660,9 @@
         <v>77</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="30">
-      <c r="A18" s="7"/>
-      <c r="B18" s="16"/>
+    <row r="18" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="12"/>
+      <c r="B18" s="11"/>
       <c r="C18" s="4" t="s">
         <v>84</v>
       </c>
@@ -2613,9 +2670,9 @@
         <v>85</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="30">
-      <c r="A19" s="7"/>
-      <c r="B19" s="16"/>
+    <row r="19" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="12"/>
+      <c r="B19" s="11"/>
       <c r="C19" s="4" t="s">
         <v>75</v>
       </c>
@@ -2623,11 +2680,11 @@
         <v>86</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="45">
-      <c r="A21" s="7" t="s">
+    <row r="21" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A21" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="B21" s="16" t="s">
+      <c r="B21" s="11" t="s">
         <v>9</v>
       </c>
       <c r="C21" s="5" t="s">
@@ -2637,9 +2694,9 @@
         <v>76</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="45">
-      <c r="A22" s="7"/>
-      <c r="B22" s="16"/>
+    <row r="22" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A22" s="12"/>
+      <c r="B22" s="11"/>
       <c r="C22" s="5" t="s">
         <v>71</v>
       </c>
@@ -2647,18 +2704,18 @@
         <v>77</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
-      <c r="A23" s="7"/>
-      <c r="B23" s="16"/>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="12"/>
+      <c r="B23" s="11"/>
       <c r="C23" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="45">
-      <c r="A25" s="7" t="s">
+    <row r="25" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A25" s="12" t="s">
         <v>89</v>
       </c>
-      <c r="B25" s="16" t="s">
+      <c r="B25" s="11" t="s">
         <v>17</v>
       </c>
       <c r="C25" s="5" t="s">
@@ -2668,9 +2725,9 @@
         <v>76</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="45">
-      <c r="A26" s="7"/>
-      <c r="B26" s="16"/>
+    <row r="26" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A26" s="12"/>
+      <c r="B26" s="11"/>
       <c r="C26" s="5" t="s">
         <v>71</v>
       </c>
@@ -2678,9 +2735,9 @@
         <v>77</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="30">
-      <c r="A27" s="7"/>
-      <c r="B27" s="16"/>
+    <row r="27" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="12"/>
+      <c r="B27" s="11"/>
       <c r="C27" s="5" t="s">
         <v>91</v>
       </c>
@@ -2688,9 +2745,9 @@
         <v>90</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="30">
-      <c r="A28" s="7"/>
-      <c r="B28" s="16"/>
+    <row r="28" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="12"/>
+      <c r="B28" s="11"/>
       <c r="C28" s="5" t="s">
         <v>92</v>
       </c>
@@ -2698,11 +2755,11 @@
         <v>93</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="45">
-      <c r="A30" s="7" t="s">
+    <row r="30" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A30" s="12" t="s">
         <v>94</v>
       </c>
-      <c r="B30" s="16" t="s">
+      <c r="B30" s="11" t="s">
         <v>38</v>
       </c>
       <c r="C30" s="5" t="s">
@@ -2712,9 +2769,9 @@
         <v>76</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="45">
-      <c r="A31" s="7"/>
-      <c r="B31" s="16"/>
+    <row r="31" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A31" s="12"/>
+      <c r="B31" s="11"/>
       <c r="C31" s="5" t="s">
         <v>71</v>
       </c>
@@ -2722,9 +2779,9 @@
         <v>77</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="30">
-      <c r="A32" s="7"/>
-      <c r="B32" s="16"/>
+    <row r="32" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A32" s="12"/>
+      <c r="B32" s="11"/>
       <c r="C32" s="5" t="s">
         <v>91</v>
       </c>
@@ -2732,9 +2789,9 @@
         <v>90</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="30">
-      <c r="A33" s="7"/>
-      <c r="B33" s="16"/>
+    <row r="33" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A33" s="12"/>
+      <c r="B33" s="11"/>
       <c r="C33" s="5" t="s">
         <v>96</v>
       </c>
@@ -2742,11 +2799,11 @@
         <v>95</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="45">
-      <c r="A35" s="7" t="s">
+    <row r="35" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A35" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="B35" s="16" t="s">
+      <c r="B35" s="11" t="s">
         <v>40</v>
       </c>
       <c r="C35" s="5" t="s">
@@ -2756,9 +2813,9 @@
         <v>76</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="45">
-      <c r="A36" s="7"/>
-      <c r="B36" s="16"/>
+    <row r="36" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A36" s="12"/>
+      <c r="B36" s="11"/>
       <c r="C36" s="5" t="s">
         <v>71</v>
       </c>
@@ -2766,9 +2823,9 @@
         <v>77</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="30">
-      <c r="A37" s="7"/>
-      <c r="B37" s="16"/>
+    <row r="37" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A37" s="12"/>
+      <c r="B37" s="11"/>
       <c r="C37" s="5" t="s">
         <v>91</v>
       </c>
@@ -2776,9 +2833,9 @@
         <v>90</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="30">
-      <c r="A38" s="7"/>
-      <c r="B38" s="16"/>
+    <row r="38" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A38" s="12"/>
+      <c r="B38" s="11"/>
       <c r="C38" s="5" t="s">
         <v>101</v>
       </c>
@@ -2786,11 +2843,11 @@
         <v>102</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="45">
-      <c r="A40" s="7" t="s">
+    <row r="40" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A40" s="12" t="s">
         <v>100</v>
       </c>
-      <c r="B40" s="16" t="s">
+      <c r="B40" s="11" t="s">
         <v>39</v>
       </c>
       <c r="C40" s="5" t="s">
@@ -2800,9 +2857,9 @@
         <v>76</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="45">
-      <c r="A41" s="7"/>
-      <c r="B41" s="16"/>
+    <row r="41" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A41" s="12"/>
+      <c r="B41" s="11"/>
       <c r="C41" s="5" t="s">
         <v>71</v>
       </c>
@@ -2810,9 +2867,9 @@
         <v>77</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="30">
-      <c r="A42" s="7"/>
-      <c r="B42" s="16"/>
+    <row r="42" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A42" s="12"/>
+      <c r="B42" s="11"/>
       <c r="C42" s="5" t="s">
         <v>91</v>
       </c>
@@ -2820,9 +2877,9 @@
         <v>90</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="30">
-      <c r="A43" s="7"/>
-      <c r="B43" s="16"/>
+    <row r="43" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A43" s="12"/>
+      <c r="B43" s="11"/>
       <c r="C43" s="5" t="s">
         <v>98</v>
       </c>
@@ -2830,11 +2887,11 @@
         <v>99</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="45">
-      <c r="A45" s="7" t="s">
+    <row r="45" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A45" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="B45" s="16" t="s">
+      <c r="B45" s="11" t="s">
         <v>16</v>
       </c>
       <c r="C45" s="5" t="s">
@@ -2844,9 +2901,9 @@
         <v>76</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="45">
-      <c r="A46" s="7"/>
-      <c r="B46" s="16"/>
+    <row r="46" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A46" s="12"/>
+      <c r="B46" s="11"/>
       <c r="C46" s="5" t="s">
         <v>71</v>
       </c>
@@ -2854,9 +2911,9 @@
         <v>77</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="30">
-      <c r="A47" s="7"/>
-      <c r="B47" s="16"/>
+    <row r="47" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A47" s="12"/>
+      <c r="B47" s="11"/>
       <c r="C47" s="5" t="s">
         <v>104</v>
       </c>
@@ -2864,9 +2921,9 @@
         <v>105</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="45">
-      <c r="A48" s="7"/>
-      <c r="B48" s="16"/>
+    <row r="48" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A48" s="12"/>
+      <c r="B48" s="11"/>
       <c r="C48" s="5" t="s">
         <v>106</v>
       </c>
@@ -2874,11 +2931,11 @@
         <v>107</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="45">
-      <c r="A50" s="7" t="s">
+    <row r="50" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A50" s="12" t="s">
         <v>108</v>
       </c>
-      <c r="B50" s="16" t="s">
+      <c r="B50" s="11" t="s">
         <v>10</v>
       </c>
       <c r="C50" s="5" t="s">
@@ -2888,9 +2945,9 @@
         <v>76</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="45">
-      <c r="A51" s="7"/>
-      <c r="B51" s="16"/>
+    <row r="51" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A51" s="12"/>
+      <c r="B51" s="11"/>
       <c r="C51" s="5" t="s">
         <v>71</v>
       </c>
@@ -2898,9 +2955,9 @@
         <v>77</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="30">
-      <c r="A52" s="7"/>
-      <c r="B52" s="16"/>
+    <row r="52" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A52" s="12"/>
+      <c r="B52" s="11"/>
       <c r="C52" s="5" t="s">
         <v>104</v>
       </c>
@@ -2908,9 +2965,9 @@
         <v>105</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="45">
-      <c r="A53" s="7"/>
-      <c r="B53" s="16"/>
+    <row r="53" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A53" s="12"/>
+      <c r="B53" s="11"/>
       <c r="C53" s="5" t="s">
         <v>109</v>
       </c>
@@ -2918,11 +2975,11 @@
         <v>110</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="45">
-      <c r="A55" s="7" t="s">
+    <row r="55" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A55" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="B55" s="16" t="s">
+      <c r="B55" s="11" t="s">
         <v>15</v>
       </c>
       <c r="C55" s="5" t="s">
@@ -2932,9 +2989,9 @@
         <v>76</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="45">
-      <c r="A56" s="7"/>
-      <c r="B56" s="16"/>
+    <row r="56" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A56" s="12"/>
+      <c r="B56" s="11"/>
       <c r="C56" s="5" t="s">
         <v>71</v>
       </c>
@@ -2942,9 +2999,9 @@
         <v>77</v>
       </c>
     </row>
-    <row r="57" spans="1:4" ht="30">
-      <c r="A57" s="7"/>
-      <c r="B57" s="16"/>
+    <row r="57" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A57" s="12"/>
+      <c r="B57" s="11"/>
       <c r="C57" s="5" t="s">
         <v>112</v>
       </c>
@@ -2952,9 +3009,9 @@
         <v>113</v>
       </c>
     </row>
-    <row r="58" spans="1:4" ht="30">
-      <c r="A58" s="7"/>
-      <c r="B58" s="16"/>
+    <row r="58" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A58" s="12"/>
+      <c r="B58" s="11"/>
       <c r="C58" s="5" t="s">
         <v>115</v>
       </c>
@@ -2962,11 +3019,11 @@
         <v>114</v>
       </c>
     </row>
-    <row r="60" spans="1:4" ht="45">
-      <c r="A60" s="11" t="s">
+    <row r="60" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A60" s="13" t="s">
         <v>116</v>
       </c>
-      <c r="B60" s="16" t="s">
+      <c r="B60" s="11" t="s">
         <v>14</v>
       </c>
       <c r="C60" s="5" t="s">
@@ -2976,9 +3033,9 @@
         <v>76</v>
       </c>
     </row>
-    <row r="61" spans="1:4" ht="45">
-      <c r="A61" s="11"/>
-      <c r="B61" s="16"/>
+    <row r="61" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A61" s="13"/>
+      <c r="B61" s="11"/>
       <c r="C61" s="5" t="s">
         <v>71</v>
       </c>
@@ -2986,9 +3043,9 @@
         <v>77</v>
       </c>
     </row>
-    <row r="62" spans="1:4" ht="30">
-      <c r="A62" s="11"/>
-      <c r="B62" s="16"/>
+    <row r="62" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A62" s="13"/>
+      <c r="B62" s="11"/>
       <c r="C62" s="5" t="s">
         <v>117</v>
       </c>
@@ -2996,9 +3053,9 @@
         <v>118</v>
       </c>
     </row>
-    <row r="63" spans="1:4" ht="30">
-      <c r="A63" s="11"/>
-      <c r="B63" s="16"/>
+    <row r="63" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A63" s="13"/>
+      <c r="B63" s="11"/>
       <c r="C63" s="5" t="s">
         <v>115</v>
       </c>
@@ -3006,11 +3063,11 @@
         <v>114</v>
       </c>
     </row>
-    <row r="65" spans="1:4" ht="45">
-      <c r="A65" s="11" t="s">
+    <row r="65" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A65" s="13" t="s">
         <v>119</v>
       </c>
-      <c r="B65" s="16" t="s">
+      <c r="B65" s="11" t="s">
         <v>19</v>
       </c>
       <c r="C65" s="5" t="s">
@@ -3020,9 +3077,9 @@
         <v>76</v>
       </c>
     </row>
-    <row r="66" spans="1:4" ht="45">
-      <c r="A66" s="11"/>
-      <c r="B66" s="16"/>
+    <row r="66" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A66" s="13"/>
+      <c r="B66" s="11"/>
       <c r="C66" s="5" t="s">
         <v>71</v>
       </c>
@@ -3030,9 +3087,9 @@
         <v>77</v>
       </c>
     </row>
-    <row r="67" spans="1:4" ht="30">
-      <c r="A67" s="11"/>
-      <c r="B67" s="16"/>
+    <row r="67" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A67" s="13"/>
+      <c r="B67" s="11"/>
       <c r="C67" s="5" t="s">
         <v>120</v>
       </c>
@@ -3040,9 +3097,9 @@
         <v>121</v>
       </c>
     </row>
-    <row r="68" spans="1:4" ht="45">
-      <c r="A68" s="11"/>
-      <c r="B68" s="16"/>
+    <row r="68" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A68" s="13"/>
+      <c r="B68" s="11"/>
       <c r="C68" s="5" t="s">
         <v>122</v>
       </c>
@@ -3050,11 +3107,11 @@
         <v>123</v>
       </c>
     </row>
-    <row r="70" spans="1:4" ht="45">
-      <c r="A70" s="7" t="s">
+    <row r="70" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A70" s="12" t="s">
         <v>124</v>
       </c>
-      <c r="B70" s="16" t="s">
+      <c r="B70" s="11" t="s">
         <v>20</v>
       </c>
       <c r="C70" s="5" t="s">
@@ -3064,9 +3121,9 @@
         <v>76</v>
       </c>
     </row>
-    <row r="71" spans="1:4" ht="45">
-      <c r="A71" s="7"/>
-      <c r="B71" s="16"/>
+    <row r="71" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A71" s="12"/>
+      <c r="B71" s="11"/>
       <c r="C71" s="5" t="s">
         <v>71</v>
       </c>
@@ -3074,9 +3131,9 @@
         <v>77</v>
       </c>
     </row>
-    <row r="72" spans="1:4" ht="45">
-      <c r="A72" s="7"/>
-      <c r="B72" s="16"/>
+    <row r="72" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A72" s="12"/>
+      <c r="B72" s="11"/>
       <c r="C72" s="5" t="s">
         <v>125</v>
       </c>
@@ -3084,9 +3141,9 @@
         <v>126</v>
       </c>
     </row>
-    <row r="73" spans="1:4" ht="45">
-      <c r="A73" s="7"/>
-      <c r="B73" s="16"/>
+    <row r="73" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A73" s="12"/>
+      <c r="B73" s="11"/>
       <c r="C73" s="5" t="s">
         <v>122</v>
       </c>
@@ -3094,11 +3151,11 @@
         <v>123</v>
       </c>
     </row>
-    <row r="75" spans="1:4" ht="45">
-      <c r="A75" s="7" t="s">
+    <row r="75" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A75" s="12" t="s">
         <v>127</v>
       </c>
-      <c r="B75" s="16" t="s">
+      <c r="B75" s="11" t="s">
         <v>41</v>
       </c>
       <c r="C75" s="5" t="s">
@@ -3108,9 +3165,9 @@
         <v>76</v>
       </c>
     </row>
-    <row r="76" spans="1:4" ht="45">
-      <c r="A76" s="7"/>
-      <c r="B76" s="16"/>
+    <row r="76" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A76" s="12"/>
+      <c r="B76" s="11"/>
       <c r="C76" s="5" t="s">
         <v>71</v>
       </c>
@@ -3118,9 +3175,9 @@
         <v>77</v>
       </c>
     </row>
-    <row r="77" spans="1:4" ht="45">
-      <c r="A77" s="7"/>
-      <c r="B77" s="16"/>
+    <row r="77" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A77" s="12"/>
+      <c r="B77" s="11"/>
       <c r="C77" s="5" t="s">
         <v>130</v>
       </c>
@@ -3128,9 +3185,9 @@
         <v>128</v>
       </c>
     </row>
-    <row r="78" spans="1:4" ht="30">
-      <c r="A78" s="7"/>
-      <c r="B78" s="16"/>
+    <row r="78" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A78" s="12"/>
+      <c r="B78" s="11"/>
       <c r="C78" s="5" t="s">
         <v>131</v>
       </c>
@@ -3138,7 +3195,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="79" spans="1:4" ht="30">
+    <row r="79" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="C79" s="5" t="s">
         <v>134</v>
       </c>
@@ -3146,11 +3203,11 @@
         <v>133</v>
       </c>
     </row>
-    <row r="80" spans="1:4" ht="45">
-      <c r="A80" s="7" t="s">
+    <row r="80" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A80" s="12" t="s">
         <v>132</v>
       </c>
-      <c r="B80" s="16" t="s">
+      <c r="B80" s="11" t="s">
         <v>22</v>
       </c>
       <c r="C80" s="5" t="s">
@@ -3160,9 +3217,9 @@
         <v>76</v>
       </c>
     </row>
-    <row r="81" spans="1:4" ht="45">
-      <c r="A81" s="7"/>
-      <c r="B81" s="16"/>
+    <row r="81" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A81" s="12"/>
+      <c r="B81" s="11"/>
       <c r="C81" s="5" t="s">
         <v>71</v>
       </c>
@@ -3170,9 +3227,9 @@
         <v>77</v>
       </c>
     </row>
-    <row r="82" spans="1:4" ht="30">
-      <c r="A82" s="7"/>
-      <c r="B82" s="16"/>
+    <row r="82" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A82" s="12"/>
+      <c r="B82" s="11"/>
       <c r="C82" s="5" t="s">
         <v>136</v>
       </c>
@@ -3180,9 +3237,9 @@
         <v>137</v>
       </c>
     </row>
-    <row r="83" spans="1:4" ht="30">
-      <c r="A83" s="7"/>
-      <c r="B83" s="16"/>
+    <row r="83" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A83" s="12"/>
+      <c r="B83" s="11"/>
       <c r="C83" s="5" t="s">
         <v>135</v>
       </c>
@@ -3190,9 +3247,9 @@
         <v>138</v>
       </c>
     </row>
-    <row r="84" spans="1:4" ht="30">
-      <c r="A84" s="7"/>
-      <c r="B84" s="16"/>
+    <row r="84" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A84" s="12"/>
+      <c r="B84" s="11"/>
       <c r="C84" s="5" t="s">
         <v>134</v>
       </c>
@@ -3200,11 +3257,11 @@
         <v>139</v>
       </c>
     </row>
-    <row r="85" spans="1:4" ht="45">
-      <c r="A85" s="7" t="s">
+    <row r="85" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A85" s="12" t="s">
         <v>140</v>
       </c>
-      <c r="B85" s="16" t="s">
+      <c r="B85" s="11" t="s">
         <v>26</v>
       </c>
       <c r="C85" s="5" t="s">
@@ -3214,9 +3271,9 @@
         <v>76</v>
       </c>
     </row>
-    <row r="86" spans="1:4" ht="45">
-      <c r="A86" s="7"/>
-      <c r="B86" s="16"/>
+    <row r="86" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A86" s="12"/>
+      <c r="B86" s="11"/>
       <c r="C86" s="5" t="s">
         <v>71</v>
       </c>
@@ -3224,9 +3281,9 @@
         <v>77</v>
       </c>
     </row>
-    <row r="87" spans="1:4" ht="30">
-      <c r="A87" s="7"/>
-      <c r="B87" s="16"/>
+    <row r="87" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A87" s="12"/>
+      <c r="B87" s="11"/>
       <c r="C87" s="5" t="s">
         <v>143</v>
       </c>
@@ -3234,11 +3291,11 @@
         <v>141</v>
       </c>
     </row>
-    <row r="89" spans="1:4" ht="45">
-      <c r="A89" s="7" t="s">
+    <row r="89" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A89" s="12" t="s">
         <v>142</v>
       </c>
-      <c r="B89" s="16" t="s">
+      <c r="B89" s="11" t="s">
         <v>23</v>
       </c>
       <c r="C89" s="5" t="s">
@@ -3248,9 +3305,9 @@
         <v>76</v>
       </c>
     </row>
-    <row r="90" spans="1:4" ht="45">
-      <c r="A90" s="7"/>
-      <c r="B90" s="16"/>
+    <row r="90" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A90" s="12"/>
+      <c r="B90" s="11"/>
       <c r="C90" s="5" t="s">
         <v>71</v>
       </c>
@@ -3258,9 +3315,9 @@
         <v>77</v>
       </c>
     </row>
-    <row r="91" spans="1:4" ht="30">
-      <c r="A91" s="7"/>
-      <c r="B91" s="16"/>
+    <row r="91" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A91" s="12"/>
+      <c r="B91" s="11"/>
       <c r="C91" s="5" t="s">
         <v>143</v>
       </c>
@@ -3268,9 +3325,9 @@
         <v>141</v>
       </c>
     </row>
-    <row r="92" spans="1:4" ht="45">
-      <c r="A92" s="7"/>
-      <c r="B92" s="16"/>
+    <row r="92" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A92" s="12"/>
+      <c r="B92" s="11"/>
       <c r="C92" s="5" t="s">
         <v>147</v>
       </c>
@@ -3278,9 +3335,9 @@
         <v>144</v>
       </c>
     </row>
-    <row r="93" spans="1:4" ht="30">
-      <c r="A93" s="7"/>
-      <c r="B93" s="16"/>
+    <row r="93" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A93" s="12"/>
+      <c r="B93" s="11"/>
       <c r="C93" s="5" t="s">
         <v>148</v>
       </c>
@@ -3288,9 +3345,9 @@
         <v>145</v>
       </c>
     </row>
-    <row r="94" spans="1:4" ht="30">
-      <c r="A94" s="7"/>
-      <c r="B94" s="16"/>
+    <row r="94" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A94" s="12"/>
+      <c r="B94" s="11"/>
       <c r="C94" s="5" t="s">
         <v>149</v>
       </c>
@@ -3298,9 +3355,9 @@
         <v>146</v>
       </c>
     </row>
-    <row r="95" spans="1:4" ht="60">
-      <c r="A95" s="7"/>
-      <c r="B95" s="16"/>
+    <row r="95" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A95" s="12"/>
+      <c r="B95" s="11"/>
       <c r="C95" s="5" t="s">
         <v>151</v>
       </c>
@@ -3308,11 +3365,11 @@
         <v>150</v>
       </c>
     </row>
-    <row r="97" spans="1:4" ht="45">
-      <c r="A97" s="7" t="s">
+    <row r="97" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A97" s="12" t="s">
         <v>152</v>
       </c>
-      <c r="B97" s="16" t="s">
+      <c r="B97" s="11" t="s">
         <v>42</v>
       </c>
       <c r="C97" s="5" t="s">
@@ -3322,9 +3379,9 @@
         <v>76</v>
       </c>
     </row>
-    <row r="98" spans="1:4" ht="45">
-      <c r="A98" s="7"/>
-      <c r="B98" s="16"/>
+    <row r="98" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A98" s="12"/>
+      <c r="B98" s="11"/>
       <c r="C98" s="5" t="s">
         <v>71</v>
       </c>
@@ -3332,9 +3389,9 @@
         <v>77</v>
       </c>
     </row>
-    <row r="99" spans="1:4" ht="30">
-      <c r="A99" s="7"/>
-      <c r="B99" s="16"/>
+    <row r="99" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A99" s="12"/>
+      <c r="B99" s="11"/>
       <c r="C99" s="5" t="s">
         <v>143</v>
       </c>
@@ -3342,9 +3399,9 @@
         <v>141</v>
       </c>
     </row>
-    <row r="100" spans="1:4" ht="45">
-      <c r="A100" s="7"/>
-      <c r="B100" s="16"/>
+    <row r="100" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A100" s="12"/>
+      <c r="B100" s="11"/>
       <c r="C100" s="5" t="s">
         <v>147</v>
       </c>
@@ -3352,9 +3409,9 @@
         <v>144</v>
       </c>
     </row>
-    <row r="101" spans="1:4" ht="30">
-      <c r="A101" s="7"/>
-      <c r="B101" s="16"/>
+    <row r="101" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A101" s="12"/>
+      <c r="B101" s="11"/>
       <c r="C101" s="5" t="s">
         <v>148</v>
       </c>
@@ -3362,9 +3419,9 @@
         <v>145</v>
       </c>
     </row>
-    <row r="102" spans="1:4" ht="30">
-      <c r="A102" s="7"/>
-      <c r="B102" s="16"/>
+    <row r="102" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A102" s="12"/>
+      <c r="B102" s="11"/>
       <c r="C102" s="5" t="s">
         <v>149</v>
       </c>
@@ -3372,9 +3429,9 @@
         <v>146</v>
       </c>
     </row>
-    <row r="103" spans="1:4" ht="75">
-      <c r="A103" s="7"/>
-      <c r="B103" s="16"/>
+    <row r="103" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A103" s="12"/>
+      <c r="B103" s="11"/>
       <c r="C103" s="5" t="s">
         <v>153</v>
       </c>
@@ -3382,11 +3439,11 @@
         <v>154</v>
       </c>
     </row>
-    <row r="105" spans="1:4" ht="45">
-      <c r="A105" s="7" t="s">
+    <row r="105" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A105" s="12" t="s">
         <v>155</v>
       </c>
-      <c r="B105" s="16" t="s">
+      <c r="B105" s="11" t="s">
         <v>24</v>
       </c>
       <c r="C105" s="5" t="s">
@@ -3396,9 +3453,9 @@
         <v>76</v>
       </c>
     </row>
-    <row r="106" spans="1:4" ht="45">
-      <c r="A106" s="7"/>
-      <c r="B106" s="16"/>
+    <row r="106" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A106" s="12"/>
+      <c r="B106" s="11"/>
       <c r="C106" s="5" t="s">
         <v>71</v>
       </c>
@@ -3406,9 +3463,9 @@
         <v>77</v>
       </c>
     </row>
-    <row r="107" spans="1:4" ht="30">
-      <c r="A107" s="7"/>
-      <c r="B107" s="16"/>
+    <row r="107" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A107" s="12"/>
+      <c r="B107" s="11"/>
       <c r="C107" s="5" t="s">
         <v>143</v>
       </c>
@@ -3416,9 +3473,9 @@
         <v>141</v>
       </c>
     </row>
-    <row r="108" spans="1:4" ht="30">
-      <c r="A108" s="7"/>
-      <c r="B108" s="16"/>
+    <row r="108" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A108" s="12"/>
+      <c r="B108" s="11"/>
       <c r="C108" s="5" t="s">
         <v>156</v>
       </c>
@@ -3426,9 +3483,9 @@
         <v>157</v>
       </c>
     </row>
-    <row r="109" spans="1:4" ht="30">
-      <c r="A109" s="7"/>
-      <c r="B109" s="16"/>
+    <row r="109" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A109" s="12"/>
+      <c r="B109" s="11"/>
       <c r="C109" s="5" t="s">
         <v>158</v>
       </c>
@@ -3436,9 +3493,9 @@
         <v>159</v>
       </c>
     </row>
-    <row r="110" spans="1:4" ht="30">
-      <c r="A110" s="7"/>
-      <c r="B110" s="16"/>
+    <row r="110" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A110" s="12"/>
+      <c r="B110" s="11"/>
       <c r="C110" s="5" t="s">
         <v>160</v>
       </c>
@@ -3446,11 +3503,11 @@
         <v>161</v>
       </c>
     </row>
-    <row r="112" spans="1:4" ht="45">
-      <c r="A112" s="7" t="s">
+    <row r="112" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A112" s="12" t="s">
         <v>171</v>
       </c>
-      <c r="B112" s="16" t="s">
+      <c r="B112" s="11" t="s">
         <v>162</v>
       </c>
       <c r="C112" s="5" t="s">
@@ -3460,9 +3517,9 @@
         <v>76</v>
       </c>
     </row>
-    <row r="113" spans="1:4" ht="45">
-      <c r="A113" s="7"/>
-      <c r="B113" s="16"/>
+    <row r="113" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A113" s="12"/>
+      <c r="B113" s="11"/>
       <c r="C113" s="5" t="s">
         <v>71</v>
       </c>
@@ -3470,9 +3527,9 @@
         <v>77</v>
       </c>
     </row>
-    <row r="114" spans="1:4" ht="30">
-      <c r="A114" s="7"/>
-      <c r="B114" s="16"/>
+    <row r="114" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A114" s="12"/>
+      <c r="B114" s="11"/>
       <c r="C114" s="5" t="s">
         <v>143</v>
       </c>
@@ -3480,9 +3537,9 @@
         <v>141</v>
       </c>
     </row>
-    <row r="115" spans="1:4" ht="30">
-      <c r="A115" s="7"/>
-      <c r="B115" s="16"/>
+    <row r="115" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A115" s="12"/>
+      <c r="B115" s="11"/>
       <c r="C115" s="5" t="s">
         <v>170</v>
       </c>
@@ -3490,9 +3547,9 @@
         <v>157</v>
       </c>
     </row>
-    <row r="116" spans="1:4" ht="30">
-      <c r="A116" s="7"/>
-      <c r="B116" s="16"/>
+    <row r="116" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A116" s="12"/>
+      <c r="B116" s="11"/>
       <c r="C116" s="5" t="s">
         <v>168</v>
       </c>
@@ -3500,9 +3557,9 @@
         <v>159</v>
       </c>
     </row>
-    <row r="117" spans="1:4" ht="60">
-      <c r="A117" s="7"/>
-      <c r="B117" s="16"/>
+    <row r="117" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A117" s="12"/>
+      <c r="B117" s="11"/>
       <c r="C117" s="5" t="s">
         <v>169</v>
       </c>
@@ -3510,11 +3567,11 @@
         <v>167</v>
       </c>
     </row>
-    <row r="119" spans="1:4" ht="45">
-      <c r="A119" s="7" t="s">
+    <row r="119" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A119" s="12" t="s">
         <v>172</v>
       </c>
-      <c r="B119" s="16" t="s">
+      <c r="B119" s="11" t="s">
         <v>166</v>
       </c>
       <c r="C119" s="5" t="s">
@@ -3524,9 +3581,9 @@
         <v>76</v>
       </c>
     </row>
-    <row r="120" spans="1:4" ht="45">
-      <c r="A120" s="7"/>
-      <c r="B120" s="16"/>
+    <row r="120" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A120" s="12"/>
+      <c r="B120" s="11"/>
       <c r="C120" s="5" t="s">
         <v>71</v>
       </c>
@@ -3534,9 +3591,9 @@
         <v>77</v>
       </c>
     </row>
-    <row r="121" spans="1:4" ht="30">
-      <c r="A121" s="7"/>
-      <c r="B121" s="16"/>
+    <row r="121" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A121" s="12"/>
+      <c r="B121" s="11"/>
       <c r="C121" s="5" t="s">
         <v>143</v>
       </c>
@@ -3544,9 +3601,9 @@
         <v>141</v>
       </c>
     </row>
-    <row r="122" spans="1:4" ht="75">
-      <c r="A122" s="7"/>
-      <c r="B122" s="16"/>
+    <row r="122" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A122" s="12"/>
+      <c r="B122" s="11"/>
       <c r="C122" s="5" t="s">
         <v>174</v>
       </c>
@@ -3554,11 +3611,11 @@
         <v>173</v>
       </c>
     </row>
-    <row r="124" spans="1:4" ht="45">
-      <c r="A124" s="7" t="s">
+    <row r="124" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A124" s="12" t="s">
         <v>175</v>
       </c>
-      <c r="B124" s="16" t="s">
+      <c r="B124" s="11" t="s">
         <v>25</v>
       </c>
       <c r="C124" s="5" t="s">
@@ -3568,9 +3625,9 @@
         <v>76</v>
       </c>
     </row>
-    <row r="125" spans="1:4" ht="45">
-      <c r="A125" s="7"/>
-      <c r="B125" s="16"/>
+    <row r="125" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A125" s="12"/>
+      <c r="B125" s="11"/>
       <c r="C125" s="5" t="s">
         <v>71</v>
       </c>
@@ -3578,9 +3635,9 @@
         <v>77</v>
       </c>
     </row>
-    <row r="126" spans="1:4" ht="30">
-      <c r="A126" s="7"/>
-      <c r="B126" s="16"/>
+    <row r="126" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A126" s="12"/>
+      <c r="B126" s="11"/>
       <c r="C126" s="5" t="s">
         <v>176</v>
       </c>
@@ -3588,11 +3645,11 @@
         <v>177</v>
       </c>
     </row>
-    <row r="127" spans="1:4" ht="45">
-      <c r="A127" s="7" t="s">
+    <row r="127" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A127" s="12" t="s">
         <v>183</v>
       </c>
-      <c r="B127" s="16" t="s">
+      <c r="B127" s="11" t="s">
         <v>27</v>
       </c>
       <c r="C127" s="5" t="s">
@@ -3602,9 +3659,9 @@
         <v>76</v>
       </c>
     </row>
-    <row r="128" spans="1:4" ht="45">
-      <c r="A128" s="7"/>
-      <c r="B128" s="16"/>
+    <row r="128" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A128" s="12"/>
+      <c r="B128" s="11"/>
       <c r="C128" s="5" t="s">
         <v>71</v>
       </c>
@@ -3612,9 +3669,9 @@
         <v>77</v>
       </c>
     </row>
-    <row r="129" spans="1:4" ht="30">
-      <c r="A129" s="7"/>
-      <c r="B129" s="16"/>
+    <row r="129" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A129" s="12"/>
+      <c r="B129" s="11"/>
       <c r="C129" s="5" t="s">
         <v>176</v>
       </c>
@@ -3622,9 +3679,9 @@
         <v>177</v>
       </c>
     </row>
-    <row r="130" spans="1:4" ht="45">
-      <c r="A130" s="7"/>
-      <c r="B130" s="16"/>
+    <row r="130" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A130" s="12"/>
+      <c r="B130" s="11"/>
       <c r="C130" s="5" t="s">
         <v>147</v>
       </c>
@@ -3632,9 +3689,9 @@
         <v>144</v>
       </c>
     </row>
-    <row r="131" spans="1:4" ht="30">
-      <c r="A131" s="7"/>
-      <c r="B131" s="16"/>
+    <row r="131" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A131" s="12"/>
+      <c r="B131" s="11"/>
       <c r="C131" s="5" t="s">
         <v>178</v>
       </c>
@@ -3642,9 +3699,9 @@
         <v>179</v>
       </c>
     </row>
-    <row r="132" spans="1:4" ht="30">
-      <c r="A132" s="7"/>
-      <c r="B132" s="16"/>
+    <row r="132" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A132" s="12"/>
+      <c r="B132" s="11"/>
       <c r="C132" s="5" t="s">
         <v>180</v>
       </c>
@@ -3652,9 +3709,9 @@
         <v>181</v>
       </c>
     </row>
-    <row r="133" spans="1:4" ht="60">
-      <c r="A133" s="7"/>
-      <c r="B133" s="16"/>
+    <row r="133" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A133" s="12"/>
+      <c r="B133" s="11"/>
       <c r="C133" s="5" t="s">
         <v>151</v>
       </c>
@@ -3662,11 +3719,11 @@
         <v>182</v>
       </c>
     </row>
-    <row r="135" spans="1:4" ht="45">
-      <c r="A135" s="7" t="s">
+    <row r="135" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A135" s="12" t="s">
         <v>186</v>
       </c>
-      <c r="B135" s="16" t="s">
+      <c r="B135" s="11" t="s">
         <v>43</v>
       </c>
       <c r="C135" s="5" t="s">
@@ -3676,9 +3733,9 @@
         <v>76</v>
       </c>
     </row>
-    <row r="136" spans="1:4" ht="45">
-      <c r="A136" s="7"/>
-      <c r="B136" s="16"/>
+    <row r="136" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A136" s="12"/>
+      <c r="B136" s="11"/>
       <c r="C136" s="5" t="s">
         <v>71</v>
       </c>
@@ -3686,9 +3743,9 @@
         <v>77</v>
       </c>
     </row>
-    <row r="137" spans="1:4" ht="30">
-      <c r="A137" s="7"/>
-      <c r="B137" s="16"/>
+    <row r="137" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A137" s="12"/>
+      <c r="B137" s="11"/>
       <c r="C137" s="5" t="s">
         <v>176</v>
       </c>
@@ -3696,9 +3753,9 @@
         <v>177</v>
       </c>
     </row>
-    <row r="138" spans="1:4" ht="45">
-      <c r="A138" s="7"/>
-      <c r="B138" s="16"/>
+    <row r="138" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A138" s="12"/>
+      <c r="B138" s="11"/>
       <c r="C138" s="5" t="s">
         <v>147</v>
       </c>
@@ -3706,9 +3763,9 @@
         <v>144</v>
       </c>
     </row>
-    <row r="139" spans="1:4" ht="30">
-      <c r="A139" s="7"/>
-      <c r="B139" s="16"/>
+    <row r="139" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A139" s="12"/>
+      <c r="B139" s="11"/>
       <c r="C139" s="5" t="s">
         <v>178</v>
       </c>
@@ -3716,9 +3773,9 @@
         <v>179</v>
       </c>
     </row>
-    <row r="140" spans="1:4" ht="30">
-      <c r="A140" s="7"/>
-      <c r="B140" s="16"/>
+    <row r="140" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A140" s="12"/>
+      <c r="B140" s="11"/>
       <c r="C140" s="5" t="s">
         <v>180</v>
       </c>
@@ -3726,9 +3783,9 @@
         <v>181</v>
       </c>
     </row>
-    <row r="141" spans="1:4" ht="30">
-      <c r="A141" s="7"/>
-      <c r="B141" s="16"/>
+    <row r="141" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A141" s="12"/>
+      <c r="B141" s="11"/>
       <c r="C141" s="5" t="s">
         <v>184</v>
       </c>
@@ -3736,11 +3793,11 @@
         <v>185</v>
       </c>
     </row>
-    <row r="143" spans="1:4" ht="45">
-      <c r="A143" s="7" t="s">
+    <row r="143" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A143" s="12" t="s">
         <v>187</v>
       </c>
-      <c r="B143" s="16" t="s">
+      <c r="B143" s="11" t="s">
         <v>28</v>
       </c>
       <c r="C143" s="5" t="s">
@@ -3750,9 +3807,9 @@
         <v>76</v>
       </c>
     </row>
-    <row r="144" spans="1:4" ht="45">
-      <c r="A144" s="7"/>
-      <c r="B144" s="16"/>
+    <row r="144" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A144" s="12"/>
+      <c r="B144" s="11"/>
       <c r="C144" s="5" t="s">
         <v>71</v>
       </c>
@@ -3760,9 +3817,9 @@
         <v>77</v>
       </c>
     </row>
-    <row r="145" spans="1:4" ht="30">
-      <c r="A145" s="7"/>
-      <c r="B145" s="16"/>
+    <row r="145" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A145" s="12"/>
+      <c r="B145" s="11"/>
       <c r="C145" s="5" t="s">
         <v>176</v>
       </c>
@@ -3770,9 +3827,9 @@
         <v>177</v>
       </c>
     </row>
-    <row r="146" spans="1:4" ht="30">
-      <c r="A146" s="7"/>
-      <c r="B146" s="16"/>
+    <row r="146" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A146" s="12"/>
+      <c r="B146" s="11"/>
       <c r="C146" s="5" t="s">
         <v>156</v>
       </c>
@@ -3780,9 +3837,9 @@
         <v>157</v>
       </c>
     </row>
-    <row r="147" spans="1:4" ht="30">
-      <c r="A147" s="7"/>
-      <c r="B147" s="16"/>
+    <row r="147" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A147" s="12"/>
+      <c r="B147" s="11"/>
       <c r="C147" s="5" t="s">
         <v>158</v>
       </c>
@@ -3790,9 +3847,9 @@
         <v>159</v>
       </c>
     </row>
-    <row r="148" spans="1:4" ht="30">
-      <c r="A148" s="7"/>
-      <c r="B148" s="16"/>
+    <row r="148" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A148" s="12"/>
+      <c r="B148" s="11"/>
       <c r="C148" s="5" t="s">
         <v>160</v>
       </c>
@@ -3800,11 +3857,11 @@
         <v>188</v>
       </c>
     </row>
-    <row r="150" spans="1:4" ht="45">
-      <c r="A150" s="7" t="s">
+    <row r="150" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A150" s="12" t="s">
         <v>189</v>
       </c>
-      <c r="B150" s="16" t="s">
+      <c r="B150" s="11" t="s">
         <v>29</v>
       </c>
       <c r="C150" s="5" t="s">
@@ -3814,9 +3871,9 @@
         <v>76</v>
       </c>
     </row>
-    <row r="151" spans="1:4" ht="45">
-      <c r="A151" s="7"/>
-      <c r="B151" s="16"/>
+    <row r="151" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A151" s="12"/>
+      <c r="B151" s="11"/>
       <c r="C151" s="5" t="s">
         <v>71</v>
       </c>
@@ -3824,9 +3881,9 @@
         <v>77</v>
       </c>
     </row>
-    <row r="152" spans="1:4" ht="30">
-      <c r="A152" s="7"/>
-      <c r="B152" s="16"/>
+    <row r="152" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A152" s="12"/>
+      <c r="B152" s="11"/>
       <c r="C152" s="5" t="s">
         <v>176</v>
       </c>
@@ -3834,9 +3891,9 @@
         <v>177</v>
       </c>
     </row>
-    <row r="153" spans="1:4" ht="60">
-      <c r="A153" s="7"/>
-      <c r="B153" s="16"/>
+    <row r="153" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A153" s="12"/>
+      <c r="B153" s="11"/>
       <c r="C153" s="5" t="s">
         <v>174</v>
       </c>
@@ -3844,11 +3901,11 @@
         <v>190</v>
       </c>
     </row>
-    <row r="155" spans="1:4" ht="45">
-      <c r="A155" s="7" t="s">
+    <row r="155" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A155" s="12" t="s">
         <v>191</v>
       </c>
-      <c r="B155" s="16" t="s">
+      <c r="B155" s="11" t="s">
         <v>30</v>
       </c>
       <c r="C155" s="5" t="s">
@@ -3858,9 +3915,9 @@
         <v>76</v>
       </c>
     </row>
-    <row r="156" spans="1:4" ht="45">
-      <c r="A156" s="7"/>
-      <c r="B156" s="16"/>
+    <row r="156" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A156" s="12"/>
+      <c r="B156" s="11"/>
       <c r="C156" s="5" t="s">
         <v>222</v>
       </c>
@@ -3868,9 +3925,9 @@
         <v>77</v>
       </c>
     </row>
-    <row r="157" spans="1:4" ht="30">
-      <c r="A157" s="7"/>
-      <c r="B157" s="16"/>
+    <row r="157" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A157" s="12"/>
+      <c r="B157" s="11"/>
       <c r="C157" s="5" t="s">
         <v>192</v>
       </c>
@@ -3878,11 +3935,11 @@
         <v>193</v>
       </c>
     </row>
-    <row r="159" spans="1:4" ht="45">
-      <c r="A159" s="7" t="s">
+    <row r="159" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A159" s="12" t="s">
         <v>194</v>
       </c>
-      <c r="B159" s="16" t="s">
+      <c r="B159" s="11" t="s">
         <v>31</v>
       </c>
       <c r="C159" s="5" t="s">
@@ -3892,9 +3949,9 @@
         <v>76</v>
       </c>
     </row>
-    <row r="160" spans="1:4" ht="45">
-      <c r="A160" s="7"/>
-      <c r="B160" s="16"/>
+    <row r="160" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A160" s="12"/>
+      <c r="B160" s="11"/>
       <c r="C160" s="5" t="s">
         <v>71</v>
       </c>
@@ -3902,9 +3959,9 @@
         <v>77</v>
       </c>
     </row>
-    <row r="161" spans="1:4" ht="30">
-      <c r="A161" s="7"/>
-      <c r="B161" s="16"/>
+    <row r="161" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A161" s="12"/>
+      <c r="B161" s="11"/>
       <c r="C161" s="5" t="s">
         <v>192</v>
       </c>
@@ -3912,9 +3969,9 @@
         <v>193</v>
       </c>
     </row>
-    <row r="162" spans="1:4" ht="45">
-      <c r="A162" s="7"/>
-      <c r="B162" s="16"/>
+    <row r="162" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A162" s="12"/>
+      <c r="B162" s="11"/>
       <c r="C162" s="5" t="s">
         <v>147</v>
       </c>
@@ -3922,9 +3979,9 @@
         <v>144</v>
       </c>
     </row>
-    <row r="163" spans="1:4" ht="45">
-      <c r="A163" s="7"/>
-      <c r="B163" s="16"/>
+    <row r="163" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A163" s="12"/>
+      <c r="B163" s="11"/>
       <c r="C163" s="5" t="s">
         <v>195</v>
       </c>
@@ -3932,9 +3989,9 @@
         <v>196</v>
       </c>
     </row>
-    <row r="164" spans="1:4" ht="60">
-      <c r="A164" s="7"/>
-      <c r="B164" s="16"/>
+    <row r="164" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A164" s="12"/>
+      <c r="B164" s="11"/>
       <c r="C164" s="5" t="s">
         <v>197</v>
       </c>
@@ -3942,11 +3999,11 @@
         <v>198</v>
       </c>
     </row>
-    <row r="166" spans="1:4" ht="45">
-      <c r="A166" s="7" t="s">
+    <row r="166" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A166" s="12" t="s">
         <v>199</v>
       </c>
-      <c r="B166" s="16" t="s">
+      <c r="B166" s="11" t="s">
         <v>44</v>
       </c>
       <c r="C166" s="5" t="s">
@@ -3956,9 +4013,9 @@
         <v>76</v>
       </c>
     </row>
-    <row r="167" spans="1:4" ht="45">
-      <c r="A167" s="7"/>
-      <c r="B167" s="16"/>
+    <row r="167" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A167" s="12"/>
+      <c r="B167" s="11"/>
       <c r="C167" s="5" t="s">
         <v>71</v>
       </c>
@@ -3966,9 +4023,9 @@
         <v>77</v>
       </c>
     </row>
-    <row r="168" spans="1:4" ht="30">
-      <c r="A168" s="7"/>
-      <c r="B168" s="16"/>
+    <row r="168" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A168" s="12"/>
+      <c r="B168" s="11"/>
       <c r="C168" s="5" t="s">
         <v>192</v>
       </c>
@@ -3976,9 +4033,9 @@
         <v>193</v>
       </c>
     </row>
-    <row r="169" spans="1:4" ht="30">
-      <c r="A169" s="7"/>
-      <c r="B169" s="16"/>
+    <row r="169" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A169" s="12"/>
+      <c r="B169" s="11"/>
       <c r="C169" s="5" t="s">
         <v>200</v>
       </c>
@@ -3986,11 +4043,11 @@
         <v>185</v>
       </c>
     </row>
-    <row r="171" spans="1:4" ht="45">
-      <c r="A171" s="7" t="s">
+    <row r="171" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A171" s="12" t="s">
         <v>201</v>
       </c>
-      <c r="B171" s="16" t="s">
+      <c r="B171" s="11" t="s">
         <v>32</v>
       </c>
       <c r="C171" s="5" t="s">
@@ -4000,9 +4057,9 @@
         <v>76</v>
       </c>
     </row>
-    <row r="172" spans="1:4" ht="45">
-      <c r="A172" s="7"/>
-      <c r="B172" s="16"/>
+    <row r="172" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A172" s="12"/>
+      <c r="B172" s="11"/>
       <c r="C172" s="5" t="s">
         <v>71</v>
       </c>
@@ -4010,9 +4067,9 @@
         <v>77</v>
       </c>
     </row>
-    <row r="173" spans="1:4" ht="30">
-      <c r="A173" s="7"/>
-      <c r="B173" s="16"/>
+    <row r="173" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A173" s="12"/>
+      <c r="B173" s="11"/>
       <c r="C173" s="5" t="s">
         <v>192</v>
       </c>
@@ -4020,9 +4077,9 @@
         <v>193</v>
       </c>
     </row>
-    <row r="174" spans="1:4" ht="30">
-      <c r="A174" s="7"/>
-      <c r="B174" s="16"/>
+    <row r="174" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A174" s="12"/>
+      <c r="B174" s="11"/>
       <c r="C174" s="5" t="s">
         <v>203</v>
       </c>
@@ -4030,9 +4087,9 @@
         <v>157</v>
       </c>
     </row>
-    <row r="175" spans="1:4" ht="30">
-      <c r="A175" s="7"/>
-      <c r="B175" s="16"/>
+    <row r="175" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A175" s="12"/>
+      <c r="B175" s="11"/>
       <c r="C175" s="5" t="s">
         <v>168</v>
       </c>
@@ -4040,9 +4097,9 @@
         <v>159</v>
       </c>
     </row>
-    <row r="176" spans="1:4" ht="60">
-      <c r="A176" s="7"/>
-      <c r="B176" s="16"/>
+    <row r="176" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A176" s="12"/>
+      <c r="B176" s="11"/>
       <c r="C176" s="5" t="s">
         <v>204</v>
       </c>
@@ -4050,11 +4107,11 @@
         <v>202</v>
       </c>
     </row>
-    <row r="178" spans="1:4" ht="45">
-      <c r="A178" s="7" t="s">
+    <row r="178" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A178" s="12" t="s">
         <v>205</v>
       </c>
-      <c r="B178" s="16" t="s">
+      <c r="B178" s="11" t="s">
         <v>33</v>
       </c>
       <c r="C178" s="5" t="s">
@@ -4064,9 +4121,9 @@
         <v>76</v>
       </c>
     </row>
-    <row r="179" spans="1:4" ht="45">
-      <c r="A179" s="7"/>
-      <c r="B179" s="16"/>
+    <row r="179" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A179" s="12"/>
+      <c r="B179" s="11"/>
       <c r="C179" s="5" t="s">
         <v>71</v>
       </c>
@@ -4074,9 +4131,9 @@
         <v>77</v>
       </c>
     </row>
-    <row r="180" spans="1:4" ht="30">
-      <c r="A180" s="7"/>
-      <c r="B180" s="16"/>
+    <row r="180" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A180" s="12"/>
+      <c r="B180" s="11"/>
       <c r="C180" s="5" t="s">
         <v>192</v>
       </c>
@@ -4084,9 +4141,9 @@
         <v>193</v>
       </c>
     </row>
-    <row r="181" spans="1:4" ht="30">
-      <c r="A181" s="7"/>
-      <c r="B181" s="16"/>
+    <row r="181" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A181" s="12"/>
+      <c r="B181" s="11"/>
       <c r="C181" s="5" t="s">
         <v>206</v>
       </c>
@@ -4094,11 +4151,11 @@
         <v>207</v>
       </c>
     </row>
-    <row r="183" spans="1:4" ht="45">
-      <c r="A183" s="7" t="s">
+    <row r="183" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A183" s="12" t="s">
         <v>208</v>
       </c>
-      <c r="B183" s="16" t="s">
+      <c r="B183" s="11" t="s">
         <v>34</v>
       </c>
       <c r="C183" s="5" t="s">
@@ -4108,9 +4165,9 @@
         <v>76</v>
       </c>
     </row>
-    <row r="184" spans="1:4" ht="45">
-      <c r="A184" s="7"/>
-      <c r="B184" s="16"/>
+    <row r="184" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A184" s="12"/>
+      <c r="B184" s="11"/>
       <c r="C184" s="5" t="s">
         <v>71</v>
       </c>
@@ -4118,9 +4175,9 @@
         <v>77</v>
       </c>
     </row>
-    <row r="185" spans="1:4" ht="45">
-      <c r="A185" s="7"/>
-      <c r="B185" s="16"/>
+    <row r="185" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A185" s="12"/>
+      <c r="B185" s="11"/>
       <c r="C185" s="5" t="s">
         <v>209</v>
       </c>
@@ -4128,11 +4185,11 @@
         <v>210</v>
       </c>
     </row>
-    <row r="186" spans="1:4" ht="45">
-      <c r="A186" s="7" t="s">
+    <row r="186" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A186" s="12" t="s">
         <v>211</v>
       </c>
-      <c r="B186" s="16" t="s">
+      <c r="B186" s="11" t="s">
         <v>35</v>
       </c>
       <c r="C186" s="5" t="s">
@@ -4142,9 +4199,9 @@
         <v>76</v>
       </c>
     </row>
-    <row r="187" spans="1:4" ht="45">
-      <c r="A187" s="7"/>
-      <c r="B187" s="16"/>
+    <row r="187" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A187" s="12"/>
+      <c r="B187" s="11"/>
       <c r="C187" s="5" t="s">
         <v>71</v>
       </c>
@@ -4152,9 +4209,9 @@
         <v>77</v>
       </c>
     </row>
-    <row r="188" spans="1:4" ht="45">
-      <c r="A188" s="7"/>
-      <c r="B188" s="16"/>
+    <row r="188" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A188" s="12"/>
+      <c r="B188" s="11"/>
       <c r="C188" s="5" t="s">
         <v>209</v>
       </c>
@@ -4162,9 +4219,9 @@
         <v>210</v>
       </c>
     </row>
-    <row r="189" spans="1:4" ht="45">
-      <c r="A189" s="7"/>
-      <c r="B189" s="16"/>
+    <row r="189" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A189" s="12"/>
+      <c r="B189" s="11"/>
       <c r="C189" s="5" t="s">
         <v>147</v>
       </c>
@@ -4172,9 +4229,9 @@
         <v>144</v>
       </c>
     </row>
-    <row r="190" spans="1:4" ht="45">
-      <c r="A190" s="7"/>
-      <c r="B190" s="16"/>
+    <row r="190" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A190" s="12"/>
+      <c r="B190" s="11"/>
       <c r="C190" s="5" t="s">
         <v>214</v>
       </c>
@@ -4182,9 +4239,9 @@
         <v>196</v>
       </c>
     </row>
-    <row r="191" spans="1:4" ht="60">
-      <c r="A191" s="7"/>
-      <c r="B191" s="16"/>
+    <row r="191" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A191" s="12"/>
+      <c r="B191" s="11"/>
       <c r="C191" s="5" t="s">
         <v>213</v>
       </c>
@@ -4192,11 +4249,11 @@
         <v>212</v>
       </c>
     </row>
-    <row r="193" spans="1:4" ht="45">
-      <c r="A193" s="7" t="s">
+    <row r="193" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A193" s="12" t="s">
         <v>215</v>
       </c>
-      <c r="B193" s="16" t="s">
+      <c r="B193" s="11" t="s">
         <v>45</v>
       </c>
       <c r="C193" s="5" t="s">
@@ -4206,9 +4263,9 @@
         <v>76</v>
       </c>
     </row>
-    <row r="194" spans="1:4" ht="45">
-      <c r="A194" s="7"/>
-      <c r="B194" s="16"/>
+    <row r="194" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A194" s="12"/>
+      <c r="B194" s="11"/>
       <c r="C194" s="5" t="s">
         <v>71</v>
       </c>
@@ -4216,9 +4273,9 @@
         <v>77</v>
       </c>
     </row>
-    <row r="195" spans="1:4" ht="45">
-      <c r="A195" s="7"/>
-      <c r="B195" s="16"/>
+    <row r="195" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A195" s="12"/>
+      <c r="B195" s="11"/>
       <c r="C195" s="5" t="s">
         <v>209</v>
       </c>
@@ -4226,9 +4283,9 @@
         <v>210</v>
       </c>
     </row>
-    <row r="196" spans="1:4" ht="30">
-      <c r="A196" s="7"/>
-      <c r="B196" s="16"/>
+    <row r="196" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A196" s="12"/>
+      <c r="B196" s="11"/>
       <c r="C196" s="5" t="s">
         <v>200</v>
       </c>
@@ -4236,11 +4293,11 @@
         <v>216</v>
       </c>
     </row>
-    <row r="198" spans="1:4" ht="45">
-      <c r="A198" s="7" t="s">
+    <row r="198" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A198" s="12" t="s">
         <v>217</v>
       </c>
-      <c r="B198" s="16" t="s">
+      <c r="B198" s="11" t="s">
         <v>36</v>
       </c>
       <c r="C198" s="5" t="s">
@@ -4250,9 +4307,9 @@
         <v>76</v>
       </c>
     </row>
-    <row r="199" spans="1:4" ht="45">
-      <c r="A199" s="7"/>
-      <c r="B199" s="16"/>
+    <row r="199" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A199" s="12"/>
+      <c r="B199" s="11"/>
       <c r="C199" s="5" t="s">
         <v>71</v>
       </c>
@@ -4260,9 +4317,9 @@
         <v>77</v>
       </c>
     </row>
-    <row r="200" spans="1:4" ht="45">
-      <c r="A200" s="7"/>
-      <c r="B200" s="16"/>
+    <row r="200" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A200" s="12"/>
+      <c r="B200" s="11"/>
       <c r="C200" s="5" t="s">
         <v>209</v>
       </c>
@@ -4270,9 +4327,9 @@
         <v>210</v>
       </c>
     </row>
-    <row r="201" spans="1:4" ht="30">
-      <c r="A201" s="7"/>
-      <c r="B201" s="16"/>
+    <row r="201" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A201" s="12"/>
+      <c r="B201" s="11"/>
       <c r="C201" s="5" t="s">
         <v>203</v>
       </c>
@@ -4280,9 +4337,9 @@
         <v>157</v>
       </c>
     </row>
-    <row r="202" spans="1:4" ht="30">
-      <c r="A202" s="7"/>
-      <c r="B202" s="16"/>
+    <row r="202" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A202" s="12"/>
+      <c r="B202" s="11"/>
       <c r="C202" s="5" t="s">
         <v>168</v>
       </c>
@@ -4290,9 +4347,9 @@
         <v>159</v>
       </c>
     </row>
-    <row r="203" spans="1:4" ht="60">
-      <c r="A203" s="7"/>
-      <c r="B203" s="16"/>
+    <row r="203" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A203" s="12"/>
+      <c r="B203" s="11"/>
       <c r="C203" s="5" t="s">
         <v>204</v>
       </c>
@@ -4300,11 +4357,11 @@
         <v>218</v>
       </c>
     </row>
-    <row r="204" spans="1:4" ht="45">
-      <c r="A204" s="7" t="s">
+    <row r="204" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A204" s="12" t="s">
         <v>219</v>
       </c>
-      <c r="B204" s="16" t="s">
+      <c r="B204" s="11" t="s">
         <v>37</v>
       </c>
       <c r="C204" s="5" t="s">
@@ -4314,9 +4371,9 @@
         <v>76</v>
       </c>
     </row>
-    <row r="205" spans="1:4" ht="45">
-      <c r="A205" s="7"/>
-      <c r="B205" s="16"/>
+    <row r="205" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A205" s="12"/>
+      <c r="B205" s="11"/>
       <c r="C205" s="5" t="s">
         <v>71</v>
       </c>
@@ -4324,9 +4381,9 @@
         <v>77</v>
       </c>
     </row>
-    <row r="206" spans="1:4" ht="45">
-      <c r="A206" s="7"/>
-      <c r="B206" s="16"/>
+    <row r="206" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A206" s="12"/>
+      <c r="B206" s="11"/>
       <c r="C206" s="5" t="s">
         <v>209</v>
       </c>
@@ -4334,9 +4391,9 @@
         <v>210</v>
       </c>
     </row>
-    <row r="207" spans="1:4" ht="30">
-      <c r="A207" s="7"/>
-      <c r="B207" s="16"/>
+    <row r="207" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A207" s="12"/>
+      <c r="B207" s="11"/>
       <c r="C207" s="5" t="s">
         <v>221</v>
       </c>
@@ -4346,44 +4403,26 @@
     </row>
   </sheetData>
   <mergeCells count="74">
-    <mergeCell ref="B186:B191"/>
-    <mergeCell ref="A186:A191"/>
-    <mergeCell ref="A21:A23"/>
-    <mergeCell ref="A155:A157"/>
-    <mergeCell ref="B155:B157"/>
-    <mergeCell ref="B198:B203"/>
-    <mergeCell ref="A198:A203"/>
-    <mergeCell ref="B204:B207"/>
-    <mergeCell ref="A204:A207"/>
-    <mergeCell ref="B193:B196"/>
-    <mergeCell ref="A193:A196"/>
-    <mergeCell ref="B97:B103"/>
-    <mergeCell ref="A97:A103"/>
-    <mergeCell ref="B55:B58"/>
-    <mergeCell ref="A55:A58"/>
-    <mergeCell ref="B60:B63"/>
-    <mergeCell ref="A60:A63"/>
-    <mergeCell ref="B65:B68"/>
-    <mergeCell ref="B150:B153"/>
-    <mergeCell ref="B178:B181"/>
-    <mergeCell ref="A178:A181"/>
-    <mergeCell ref="A183:A185"/>
-    <mergeCell ref="B183:B185"/>
-    <mergeCell ref="B159:B164"/>
-    <mergeCell ref="A159:A164"/>
-    <mergeCell ref="A166:A169"/>
-    <mergeCell ref="B166:B169"/>
-    <mergeCell ref="B171:B176"/>
-    <mergeCell ref="A171:A176"/>
-    <mergeCell ref="A150:A153"/>
-    <mergeCell ref="B124:B126"/>
-    <mergeCell ref="A124:A126"/>
-    <mergeCell ref="A127:A133"/>
-    <mergeCell ref="B143:B148"/>
-    <mergeCell ref="A143:A148"/>
-    <mergeCell ref="B127:B133"/>
-    <mergeCell ref="B135:B141"/>
-    <mergeCell ref="A135:A141"/>
+    <mergeCell ref="B30:B33"/>
+    <mergeCell ref="A30:A33"/>
+    <mergeCell ref="A2:A7"/>
+    <mergeCell ref="B2:B7"/>
+    <mergeCell ref="B9:B14"/>
+    <mergeCell ref="A9:A14"/>
+    <mergeCell ref="A16:A19"/>
+    <mergeCell ref="B16:B19"/>
+    <mergeCell ref="B21:B23"/>
+    <mergeCell ref="B25:B28"/>
+    <mergeCell ref="A25:A28"/>
+    <mergeCell ref="A65:A68"/>
+    <mergeCell ref="B35:B38"/>
+    <mergeCell ref="A35:A38"/>
+    <mergeCell ref="B40:B43"/>
+    <mergeCell ref="A40:A43"/>
+    <mergeCell ref="B50:B53"/>
+    <mergeCell ref="A50:A53"/>
+    <mergeCell ref="B45:B48"/>
+    <mergeCell ref="A45:A48"/>
     <mergeCell ref="B119:B122"/>
     <mergeCell ref="A119:A122"/>
     <mergeCell ref="B112:B117"/>
@@ -4400,26 +4439,44 @@
     <mergeCell ref="B85:B87"/>
     <mergeCell ref="B89:B95"/>
     <mergeCell ref="A89:A95"/>
-    <mergeCell ref="A65:A68"/>
-    <mergeCell ref="B35:B38"/>
-    <mergeCell ref="A35:A38"/>
-    <mergeCell ref="B40:B43"/>
-    <mergeCell ref="A40:A43"/>
-    <mergeCell ref="B50:B53"/>
-    <mergeCell ref="A50:A53"/>
-    <mergeCell ref="B45:B48"/>
-    <mergeCell ref="A45:A48"/>
-    <mergeCell ref="B30:B33"/>
-    <mergeCell ref="A30:A33"/>
-    <mergeCell ref="A2:A7"/>
-    <mergeCell ref="B2:B7"/>
-    <mergeCell ref="B9:B14"/>
-    <mergeCell ref="A9:A14"/>
-    <mergeCell ref="A16:A19"/>
-    <mergeCell ref="B16:B19"/>
-    <mergeCell ref="B21:B23"/>
-    <mergeCell ref="B25:B28"/>
-    <mergeCell ref="A25:A28"/>
+    <mergeCell ref="A150:A153"/>
+    <mergeCell ref="B124:B126"/>
+    <mergeCell ref="A124:A126"/>
+    <mergeCell ref="A127:A133"/>
+    <mergeCell ref="B143:B148"/>
+    <mergeCell ref="A143:A148"/>
+    <mergeCell ref="B127:B133"/>
+    <mergeCell ref="B135:B141"/>
+    <mergeCell ref="A135:A141"/>
+    <mergeCell ref="B183:B185"/>
+    <mergeCell ref="B159:B164"/>
+    <mergeCell ref="A159:A164"/>
+    <mergeCell ref="A166:A169"/>
+    <mergeCell ref="B166:B169"/>
+    <mergeCell ref="B171:B176"/>
+    <mergeCell ref="A171:A176"/>
+    <mergeCell ref="B198:B203"/>
+    <mergeCell ref="A198:A203"/>
+    <mergeCell ref="B204:B207"/>
+    <mergeCell ref="A204:A207"/>
+    <mergeCell ref="B193:B196"/>
+    <mergeCell ref="A193:A196"/>
+    <mergeCell ref="B186:B191"/>
+    <mergeCell ref="A186:A191"/>
+    <mergeCell ref="A21:A23"/>
+    <mergeCell ref="A155:A157"/>
+    <mergeCell ref="B155:B157"/>
+    <mergeCell ref="B97:B103"/>
+    <mergeCell ref="A97:A103"/>
+    <mergeCell ref="B55:B58"/>
+    <mergeCell ref="A55:A58"/>
+    <mergeCell ref="B60:B63"/>
+    <mergeCell ref="A60:A63"/>
+    <mergeCell ref="B65:B68"/>
+    <mergeCell ref="B150:B153"/>
+    <mergeCell ref="B178:B181"/>
+    <mergeCell ref="A178:A181"/>
+    <mergeCell ref="A183:A185"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>